<commit_message>
feat: [Export] Différents exports et correctifs
</commit_message>
<xml_diff>
--- a/public/excel/mcc_rcc.xlsx
+++ b/public/excel/mcc_rcc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidannebicque/Sites/redigeTonBut/public/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D51421D-7371-4C49-97CC-D301935DF8E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{551E8798-2B3F-284B-B080-D88BABA423E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32580" yWindow="1160" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="modele" sheetId="4" r:id="rId1"/>
@@ -189,9 +189,6 @@
 Apogée</t>
   </si>
   <si>
-    <t>Intitulé court (20 caractères)</t>
-  </si>
-  <si>
     <t>Parcours Strat-UX</t>
   </si>
   <si>
@@ -219,12 +216,15 @@
     <t>H.
 Projet</t>
   </si>
+  <si>
+    <t>Intitulé court (19 caractères)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1029,7 +1029,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="210">
+  <cellXfs count="214">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1543,6 +1543,9 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1693,7 +1696,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1701,11 +1713,132 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Pourcentage" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="16">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2179,11 +2312,11 @@
   </sheetPr>
   <dimension ref="A1:AX60"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="S32" sqref="S32"/>
+    <sheetView showGridLines="0" topLeftCell="A2" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22:D49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="12" customWidth="1"/>
     <col min="3" max="3" width="50.33203125" customWidth="1"/>
@@ -2198,7 +2331,7 @@
     <col min="44" max="48" width="11.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:44" ht="17" customHeight="1" thickBot="1">
+    <row r="1" spans="1:44" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7"/>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -2248,7 +2381,7 @@
       <c r="AQ1" s="17"/>
       <c r="AR1" s="3"/>
     </row>
-    <row r="2" spans="1:44" ht="17" customHeight="1" thickBot="1">
+    <row r="2" spans="1:44" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
@@ -2264,7 +2397,7 @@
       <c r="K2" s="145"/>
       <c r="L2" s="146"/>
       <c r="M2" s="144" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="N2" s="145"/>
       <c r="O2" s="145"/>
@@ -2296,7 +2429,7 @@
       <c r="AQ2" s="8"/>
       <c r="AR2" s="7"/>
     </row>
-    <row r="3" spans="1:44" ht="17" customHeight="1" thickBot="1">
+    <row r="3" spans="1:44" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
@@ -2312,7 +2445,7 @@
       <c r="K3" s="145"/>
       <c r="L3" s="146"/>
       <c r="M3" s="144" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="N3" s="145"/>
       <c r="O3" s="145"/>
@@ -2344,7 +2477,7 @@
       <c r="AQ3" s="8"/>
       <c r="AR3" s="7"/>
     </row>
-    <row r="4" spans="1:44" ht="17" customHeight="1" thickBot="1">
+    <row r="4" spans="1:44" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7"/>
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
@@ -2392,7 +2525,7 @@
       <c r="AQ4" s="8"/>
       <c r="AR4" s="7"/>
     </row>
-    <row r="5" spans="1:44" ht="17" customHeight="1" thickBot="1">
+    <row r="5" spans="1:44" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
@@ -2440,7 +2573,7 @@
       <c r="AQ5" s="8"/>
       <c r="AR5" s="7"/>
     </row>
-    <row r="6" spans="1:44" ht="17" customHeight="1" thickBot="1">
+    <row r="6" spans="1:44" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
       <c r="E6" s="7"/>
@@ -2486,7 +2619,7 @@
       <c r="AQ6" s="8"/>
       <c r="AR6" s="7"/>
     </row>
-    <row r="7" spans="1:44" ht="17" customHeight="1">
+    <row r="7" spans="1:44" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
@@ -2523,7 +2656,7 @@
       <c r="AJ7" s="5"/>
       <c r="AK7" s="5"/>
     </row>
-    <row r="8" spans="1:44" ht="15.5" customHeight="1">
+    <row r="8" spans="1:44" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
         <v>18</v>
       </c>
@@ -2557,7 +2690,7 @@
       <c r="AJ8" s="5"/>
       <c r="AK8" s="5"/>
     </row>
-    <row r="9" spans="1:44" ht="5" customHeight="1">
+    <row r="9" spans="1:44" ht="5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -2601,7 +2734,7 @@
       <c r="AQ9" s="17"/>
       <c r="AR9" s="5"/>
     </row>
-    <row r="10" spans="1:44" ht="15.5" customHeight="1">
+    <row r="10" spans="1:44" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="14" t="s">
@@ -2626,7 +2759,7 @@
       <c r="T10" s="6"/>
       <c r="U10" s="6"/>
     </row>
-    <row r="11" spans="1:44" ht="5" customHeight="1">
+    <row r="11" spans="1:44" ht="5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -2634,17 +2767,17 @@
       <c r="E11" s="24"/>
       <c r="F11" s="11"/>
     </row>
-    <row r="12" spans="1:44" ht="15.5" customHeight="1">
+    <row r="12" spans="1:44" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E12" s="22"/>
       <c r="F12" s="9" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:44" ht="5" customHeight="1">
+    <row r="13" spans="1:44" ht="5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E13" s="23"/>
       <c r="F13" s="9"/>
     </row>
-    <row r="14" spans="1:44" ht="15.5" customHeight="1">
+    <row r="14" spans="1:44" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -2654,7 +2787,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:44" ht="11" customHeight="1" thickBot="1">
+    <row r="15" spans="1:44" ht="11" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="152"/>
       <c r="B15" s="152"/>
       <c r="C15" s="152"/>
@@ -2662,7 +2795,7 @@
       <c r="E15" s="8"/>
       <c r="F15" s="8"/>
     </row>
-    <row r="16" spans="1:44" ht="24.75" customHeight="1" thickBot="1">
+    <row r="16" spans="1:44" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="15"/>
       <c r="B16" s="52"/>
       <c r="C16" s="55"/>
@@ -2706,7 +2839,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:43" ht="24.75" customHeight="1" thickBot="1">
+    <row r="17" spans="1:43" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="15"/>
       <c r="B17" s="52"/>
       <c r="C17" s="55"/>
@@ -2750,7 +2883,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:43" ht="45.75" customHeight="1" thickBot="1">
+    <row r="18" spans="1:43" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="15"/>
       <c r="B18" s="52"/>
       <c r="C18" s="55"/>
@@ -2792,11 +2925,11 @@
       <c r="AL18" s="141"/>
       <c r="AM18" s="142"/>
       <c r="AN18" s="30"/>
-      <c r="AO18" s="174"/>
+      <c r="AO18" s="175"/>
       <c r="AP18" s="28"/>
-      <c r="AQ18" s="168"/>
-    </row>
-    <row r="19" spans="1:43" s="2" customFormat="1" ht="45.75" customHeight="1" thickBot="1">
+      <c r="AQ18" s="169"/>
+    </row>
+    <row r="19" spans="1:43" s="2" customFormat="1" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="127" t="s">
         <v>17</v>
       </c>
@@ -2816,7 +2949,7 @@
       </c>
       <c r="L19" s="156"/>
       <c r="M19" s="156"/>
-      <c r="N19" s="163" t="s">
+      <c r="N19" s="164" t="s">
         <v>24</v>
       </c>
       <c r="O19" s="143"/>
@@ -2831,7 +2964,7 @@
       <c r="T19" s="143" t="s">
         <v>27</v>
       </c>
-      <c r="U19" s="173"/>
+      <c r="U19" s="174"/>
       <c r="V19" s="143" t="s">
         <v>25</v>
       </c>
@@ -2844,10 +2977,10 @@
         <v>38</v>
       </c>
       <c r="AA19" s="130"/>
-      <c r="AB19" s="171" t="s">
+      <c r="AB19" s="172" t="s">
         <v>34</v>
       </c>
-      <c r="AC19" s="172"/>
+      <c r="AC19" s="173"/>
       <c r="AD19" s="130" t="s">
         <v>26</v>
       </c>
@@ -2869,22 +3002,22 @@
       </c>
       <c r="AM19" s="131"/>
       <c r="AN19" s="28"/>
-      <c r="AO19" s="175"/>
+      <c r="AO19" s="176"/>
       <c r="AP19" s="28"/>
-      <c r="AQ19" s="169"/>
-    </row>
-    <row r="20" spans="1:43" ht="22.5" customHeight="1">
-      <c r="A20" s="164" t="s">
+      <c r="AQ19" s="170"/>
+    </row>
+    <row r="20" spans="1:43" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="210" t="s">
         <v>50</v>
       </c>
-      <c r="B20" s="187" t="s">
+      <c r="B20" s="188" t="s">
         <v>10</v>
       </c>
-      <c r="C20" s="166" t="s">
+      <c r="C20" s="167" t="s">
         <v>9</v>
       </c>
-      <c r="D20" s="166" t="s">
-        <v>51</v>
+      <c r="D20" s="167" t="s">
+        <v>60</v>
       </c>
       <c r="E20" s="150" t="s">
         <v>48</v>
@@ -2898,22 +3031,22 @@
       <c r="H20" s="157" t="s">
         <v>3</v>
       </c>
-      <c r="I20" s="188" t="s">
+      <c r="I20" s="189" t="s">
         <v>4</v>
       </c>
-      <c r="J20" s="209" t="s">
-        <v>60</v>
-      </c>
-      <c r="K20" s="160" t="s">
+      <c r="J20" s="159" t="s">
+        <v>59</v>
+      </c>
+      <c r="K20" s="161" t="s">
         <v>2</v>
       </c>
-      <c r="L20" s="189" t="s">
+      <c r="L20" s="190" t="s">
         <v>3</v>
       </c>
-      <c r="M20" s="186" t="s">
+      <c r="M20" s="187" t="s">
         <v>4</v>
       </c>
-      <c r="N20" s="161" t="s">
+      <c r="N20" s="162" t="s">
         <v>30</v>
       </c>
       <c r="O20" s="133" t="s">
@@ -2937,7 +3070,7 @@
       <c r="U20" s="135" t="s">
         <v>31</v>
       </c>
-      <c r="V20" s="161" t="s">
+      <c r="V20" s="162" t="s">
         <v>30</v>
       </c>
       <c r="W20" s="133" t="s">
@@ -2949,7 +3082,7 @@
       <c r="Y20" s="135" t="s">
         <v>31</v>
       </c>
-      <c r="Z20" s="161" t="s">
+      <c r="Z20" s="162" t="s">
         <v>30</v>
       </c>
       <c r="AA20" s="133" t="s">
@@ -2973,7 +3106,7 @@
       <c r="AG20" s="135" t="s">
         <v>31</v>
       </c>
-      <c r="AH20" s="161" t="s">
+      <c r="AH20" s="162" t="s">
         <v>30</v>
       </c>
       <c r="AI20" s="133" t="s">
@@ -2992,25 +3125,25 @@
         <v>31</v>
       </c>
       <c r="AN20" s="29"/>
-      <c r="AO20" s="175"/>
+      <c r="AO20" s="176"/>
       <c r="AP20" s="29"/>
-      <c r="AQ20" s="169"/>
-    </row>
-    <row r="21" spans="1:43" ht="22.5" customHeight="1" thickBot="1">
-      <c r="A21" s="165"/>
-      <c r="B21" s="165"/>
-      <c r="C21" s="167"/>
-      <c r="D21" s="167"/>
+      <c r="AQ20" s="170"/>
+    </row>
+    <row r="21" spans="1:43" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="211"/>
+      <c r="B21" s="166"/>
+      <c r="C21" s="168"/>
+      <c r="D21" s="168"/>
       <c r="E21" s="151"/>
       <c r="F21" s="151"/>
       <c r="G21" s="154"/>
       <c r="H21" s="158"/>
       <c r="I21" s="158"/>
-      <c r="J21" s="159"/>
+      <c r="J21" s="160"/>
       <c r="K21" s="154"/>
       <c r="L21" s="158"/>
-      <c r="M21" s="159"/>
-      <c r="N21" s="162"/>
+      <c r="M21" s="160"/>
+      <c r="N21" s="163"/>
       <c r="O21" s="134"/>
       <c r="P21" s="134"/>
       <c r="Q21" s="134"/>
@@ -3018,11 +3151,11 @@
       <c r="S21" s="134"/>
       <c r="T21" s="134"/>
       <c r="U21" s="136"/>
-      <c r="V21" s="162"/>
+      <c r="V21" s="163"/>
       <c r="W21" s="134"/>
       <c r="X21" s="134"/>
       <c r="Y21" s="136"/>
-      <c r="Z21" s="162"/>
+      <c r="Z21" s="163"/>
       <c r="AA21" s="134"/>
       <c r="AB21" s="134"/>
       <c r="AC21" s="134"/>
@@ -3030,22 +3163,22 @@
       <c r="AE21" s="134"/>
       <c r="AF21" s="134"/>
       <c r="AG21" s="136"/>
-      <c r="AH21" s="162"/>
+      <c r="AH21" s="163"/>
       <c r="AI21" s="134"/>
       <c r="AJ21" s="134"/>
       <c r="AK21" s="134"/>
       <c r="AL21" s="134"/>
       <c r="AM21" s="136"/>
       <c r="AN21" s="29"/>
-      <c r="AO21" s="176"/>
+      <c r="AO21" s="177"/>
       <c r="AP21" s="29"/>
-      <c r="AQ21" s="170"/>
-    </row>
-    <row r="22" spans="1:43" ht="28.25" customHeight="1">
+      <c r="AQ21" s="171"/>
+    </row>
+    <row r="22" spans="1:43" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="51"/>
       <c r="B22" s="69"/>
       <c r="C22" s="75"/>
-      <c r="D22" s="19"/>
+      <c r="D22" s="212"/>
       <c r="E22" s="45"/>
       <c r="F22" s="45"/>
       <c r="G22" s="31"/>
@@ -3086,11 +3219,11 @@
       <c r="AP22" s="35"/>
       <c r="AQ22" s="92"/>
     </row>
-    <row r="23" spans="1:43" ht="27.75" customHeight="1">
+    <row r="23" spans="1:43" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="48"/>
       <c r="B23" s="70"/>
       <c r="C23" s="76"/>
-      <c r="D23" s="20"/>
+      <c r="D23" s="212"/>
       <c r="E23" s="46"/>
       <c r="F23" s="46"/>
       <c r="G23" s="36"/>
@@ -3131,11 +3264,11 @@
       <c r="AP23" s="35"/>
       <c r="AQ23" s="39"/>
     </row>
-    <row r="24" spans="1:43" ht="28.25" customHeight="1">
+    <row r="24" spans="1:43" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="48"/>
       <c r="B24" s="70"/>
       <c r="C24" s="76"/>
-      <c r="D24" s="20"/>
+      <c r="D24" s="212"/>
       <c r="E24" s="46"/>
       <c r="F24" s="46"/>
       <c r="G24" s="36"/>
@@ -3176,11 +3309,11 @@
       <c r="AP24" s="35"/>
       <c r="AQ24" s="39"/>
     </row>
-    <row r="25" spans="1:43" ht="28.25" customHeight="1">
+    <row r="25" spans="1:43" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="48"/>
       <c r="B25" s="70"/>
       <c r="C25" s="76"/>
-      <c r="D25" s="20"/>
+      <c r="D25" s="212"/>
       <c r="E25" s="46"/>
       <c r="F25" s="46"/>
       <c r="G25" s="36"/>
@@ -3221,11 +3354,11 @@
       <c r="AP25" s="35"/>
       <c r="AQ25" s="39"/>
     </row>
-    <row r="26" spans="1:43" ht="27.75" customHeight="1">
+    <row r="26" spans="1:43" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="48"/>
       <c r="B26" s="70"/>
       <c r="C26" s="76"/>
-      <c r="D26" s="20"/>
+      <c r="D26" s="212"/>
       <c r="E26" s="46"/>
       <c r="F26" s="46"/>
       <c r="G26" s="36"/>
@@ -3266,11 +3399,11 @@
       <c r="AP26" s="35"/>
       <c r="AQ26" s="39"/>
     </row>
-    <row r="27" spans="1:43" ht="28.25" customHeight="1">
+    <row r="27" spans="1:43" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="48"/>
       <c r="B27" s="70"/>
       <c r="C27" s="76"/>
-      <c r="D27" s="20"/>
+      <c r="D27" s="212"/>
       <c r="E27" s="46"/>
       <c r="F27" s="46"/>
       <c r="G27" s="36"/>
@@ -3311,11 +3444,11 @@
       <c r="AP27" s="35"/>
       <c r="AQ27" s="39"/>
     </row>
-    <row r="28" spans="1:43" ht="27.75" customHeight="1">
+    <row r="28" spans="1:43" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="48"/>
       <c r="B28" s="70"/>
       <c r="C28" s="76"/>
-      <c r="D28" s="20"/>
+      <c r="D28" s="212"/>
       <c r="E28" s="46"/>
       <c r="F28" s="46"/>
       <c r="G28" s="36"/>
@@ -3356,11 +3489,11 @@
       <c r="AP28" s="35"/>
       <c r="AQ28" s="39"/>
     </row>
-    <row r="29" spans="1:43" ht="28.25" customHeight="1">
+    <row r="29" spans="1:43" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="48"/>
       <c r="B29" s="70"/>
       <c r="C29" s="76"/>
-      <c r="D29" s="20"/>
+      <c r="D29" s="212"/>
       <c r="E29" s="46"/>
       <c r="F29" s="46"/>
       <c r="G29" s="36"/>
@@ -3401,11 +3534,11 @@
       <c r="AP29" s="35"/>
       <c r="AQ29" s="39"/>
     </row>
-    <row r="30" spans="1:43" ht="28.25" customHeight="1">
+    <row r="30" spans="1:43" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="48"/>
       <c r="B30" s="70"/>
       <c r="C30" s="76"/>
-      <c r="D30" s="20"/>
+      <c r="D30" s="212"/>
       <c r="E30" s="46"/>
       <c r="F30" s="46"/>
       <c r="G30" s="36"/>
@@ -3446,11 +3579,11 @@
       <c r="AP30" s="35"/>
       <c r="AQ30" s="39"/>
     </row>
-    <row r="31" spans="1:43" ht="28.25" customHeight="1">
+    <row r="31" spans="1:43" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="48"/>
       <c r="B31" s="70"/>
       <c r="C31" s="76"/>
-      <c r="D31" s="20"/>
+      <c r="D31" s="212"/>
       <c r="E31" s="46"/>
       <c r="F31" s="46"/>
       <c r="G31" s="36"/>
@@ -3491,11 +3624,11 @@
       <c r="AP31" s="35"/>
       <c r="AQ31" s="39"/>
     </row>
-    <row r="32" spans="1:43" ht="28.25" customHeight="1">
+    <row r="32" spans="1:43" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="48"/>
       <c r="B32" s="70"/>
       <c r="C32" s="76"/>
-      <c r="D32" s="20"/>
+      <c r="D32" s="212"/>
       <c r="E32" s="46"/>
       <c r="F32" s="46"/>
       <c r="G32" s="36"/>
@@ -3536,11 +3669,11 @@
       <c r="AP32" s="35"/>
       <c r="AQ32" s="39"/>
     </row>
-    <row r="33" spans="1:43" ht="28.25" customHeight="1">
+    <row r="33" spans="1:43" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="48"/>
       <c r="B33" s="70"/>
       <c r="C33" s="76"/>
-      <c r="D33" s="20"/>
+      <c r="D33" s="212"/>
       <c r="E33" s="46"/>
       <c r="F33" s="46"/>
       <c r="G33" s="36"/>
@@ -3581,11 +3714,11 @@
       <c r="AP33" s="35"/>
       <c r="AQ33" s="39"/>
     </row>
-    <row r="34" spans="1:43" ht="28.25" customHeight="1">
+    <row r="34" spans="1:43" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="48"/>
       <c r="B34" s="70"/>
       <c r="C34" s="76"/>
-      <c r="D34" s="20"/>
+      <c r="D34" s="212"/>
       <c r="E34" s="46"/>
       <c r="F34" s="46"/>
       <c r="G34" s="36"/>
@@ -3626,11 +3759,11 @@
       <c r="AP34" s="35"/>
       <c r="AQ34" s="39"/>
     </row>
-    <row r="35" spans="1:43" ht="28.25" customHeight="1">
+    <row r="35" spans="1:43" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="48"/>
       <c r="B35" s="70"/>
       <c r="C35" s="76"/>
-      <c r="D35" s="20"/>
+      <c r="D35" s="212"/>
       <c r="E35" s="46"/>
       <c r="F35" s="46"/>
       <c r="G35" s="36"/>
@@ -3671,11 +3804,11 @@
       <c r="AP35" s="35"/>
       <c r="AQ35" s="39"/>
     </row>
-    <row r="36" spans="1:43" ht="28.25" customHeight="1">
+    <row r="36" spans="1:43" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="48"/>
       <c r="B36" s="70"/>
       <c r="C36" s="76"/>
-      <c r="D36" s="20"/>
+      <c r="D36" s="212"/>
       <c r="E36" s="46"/>
       <c r="F36" s="46"/>
       <c r="G36" s="36"/>
@@ -3716,11 +3849,11 @@
       <c r="AP36" s="35"/>
       <c r="AQ36" s="39"/>
     </row>
-    <row r="37" spans="1:43" ht="28.25" customHeight="1">
+    <row r="37" spans="1:43" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="48"/>
       <c r="B37" s="70"/>
       <c r="C37" s="76"/>
-      <c r="D37" s="20"/>
+      <c r="D37" s="212"/>
       <c r="E37" s="46"/>
       <c r="F37" s="46"/>
       <c r="G37" s="36"/>
@@ -3761,11 +3894,11 @@
       <c r="AP37" s="35"/>
       <c r="AQ37" s="39"/>
     </row>
-    <row r="38" spans="1:43" ht="28.25" customHeight="1">
+    <row r="38" spans="1:43" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="48"/>
       <c r="B38" s="70"/>
       <c r="C38" s="76"/>
-      <c r="D38" s="20"/>
+      <c r="D38" s="212"/>
       <c r="E38" s="46"/>
       <c r="F38" s="46"/>
       <c r="G38" s="36"/>
@@ -3806,11 +3939,11 @@
       <c r="AP38" s="35"/>
       <c r="AQ38" s="39"/>
     </row>
-    <row r="39" spans="1:43" ht="28.25" customHeight="1">
+    <row r="39" spans="1:43" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="48"/>
       <c r="B39" s="70"/>
       <c r="C39" s="76"/>
-      <c r="D39" s="20"/>
+      <c r="D39" s="212"/>
       <c r="E39" s="46"/>
       <c r="F39" s="46"/>
       <c r="G39" s="36"/>
@@ -3851,11 +3984,11 @@
       <c r="AP39" s="35"/>
       <c r="AQ39" s="39"/>
     </row>
-    <row r="40" spans="1:43" ht="28.25" customHeight="1">
+    <row r="40" spans="1:43" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="48"/>
       <c r="B40" s="70"/>
       <c r="C40" s="76"/>
-      <c r="D40" s="20"/>
+      <c r="D40" s="212"/>
       <c r="E40" s="46"/>
       <c r="F40" s="46"/>
       <c r="G40" s="36"/>
@@ -3896,11 +4029,11 @@
       <c r="AP40" s="35"/>
       <c r="AQ40" s="39"/>
     </row>
-    <row r="41" spans="1:43" ht="28.25" customHeight="1">
+    <row r="41" spans="1:43" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="48"/>
       <c r="B41" s="70"/>
       <c r="C41" s="76"/>
-      <c r="D41" s="20"/>
+      <c r="D41" s="212"/>
       <c r="E41" s="46"/>
       <c r="F41" s="46"/>
       <c r="G41" s="36"/>
@@ -3941,11 +4074,11 @@
       <c r="AP41" s="35"/>
       <c r="AQ41" s="39"/>
     </row>
-    <row r="42" spans="1:43" ht="28.25" customHeight="1">
-      <c r="A42" s="12"/>
+    <row r="42" spans="1:43" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="48"/>
       <c r="B42" s="70"/>
       <c r="C42" s="76"/>
-      <c r="D42" s="20"/>
+      <c r="D42" s="212"/>
       <c r="E42" s="46"/>
       <c r="F42" s="46"/>
       <c r="G42" s="36"/>
@@ -3986,11 +4119,11 @@
       <c r="AP42" s="35"/>
       <c r="AQ42" s="39"/>
     </row>
-    <row r="43" spans="1:43" ht="28.25" customHeight="1">
+    <row r="43" spans="1:43" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="48"/>
       <c r="B43" s="70"/>
       <c r="C43" s="76"/>
-      <c r="D43" s="20"/>
+      <c r="D43" s="212"/>
       <c r="E43" s="46"/>
       <c r="F43" s="46"/>
       <c r="G43" s="36"/>
@@ -4031,11 +4164,11 @@
       <c r="AP43" s="35"/>
       <c r="AQ43" s="39"/>
     </row>
-    <row r="44" spans="1:43" ht="28.25" customHeight="1">
-      <c r="A44" s="12"/>
+    <row r="44" spans="1:43" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="48"/>
       <c r="B44" s="70"/>
       <c r="C44" s="76"/>
-      <c r="D44" s="20"/>
+      <c r="D44" s="212"/>
       <c r="E44" s="46"/>
       <c r="F44" s="46"/>
       <c r="G44" s="36"/>
@@ -4076,11 +4209,11 @@
       <c r="AP44" s="35"/>
       <c r="AQ44" s="39"/>
     </row>
-    <row r="45" spans="1:43" ht="28.25" customHeight="1">
+    <row r="45" spans="1:43" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="48"/>
       <c r="B45" s="70"/>
       <c r="C45" s="76"/>
-      <c r="D45" s="20"/>
+      <c r="D45" s="212"/>
       <c r="E45" s="46"/>
       <c r="F45" s="46"/>
       <c r="G45" s="36"/>
@@ -4121,11 +4254,11 @@
       <c r="AP45" s="35"/>
       <c r="AQ45" s="39"/>
     </row>
-    <row r="46" spans="1:43" ht="28.25" customHeight="1">
-      <c r="A46" s="12"/>
+    <row r="46" spans="1:43" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="48"/>
       <c r="B46" s="70"/>
       <c r="C46" s="76"/>
-      <c r="D46" s="20"/>
+      <c r="D46" s="212"/>
       <c r="E46" s="46"/>
       <c r="F46" s="46"/>
       <c r="G46" s="36"/>
@@ -4166,11 +4299,11 @@
       <c r="AP46" s="35"/>
       <c r="AQ46" s="39"/>
     </row>
-    <row r="47" spans="1:43" ht="28.25" customHeight="1">
+    <row r="47" spans="1:43" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="48"/>
       <c r="B47" s="70"/>
       <c r="C47" s="76"/>
-      <c r="D47" s="20"/>
+      <c r="D47" s="212"/>
       <c r="E47" s="46"/>
       <c r="F47" s="46"/>
       <c r="G47" s="36"/>
@@ -4211,11 +4344,11 @@
       <c r="AP47" s="35"/>
       <c r="AQ47" s="39"/>
     </row>
-    <row r="48" spans="1:43" ht="27.75" customHeight="1">
-      <c r="A48" s="12"/>
+    <row r="48" spans="1:43" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="48"/>
       <c r="B48" s="70"/>
       <c r="C48" s="76"/>
-      <c r="D48" s="20"/>
+      <c r="D48" s="212"/>
       <c r="E48" s="46"/>
       <c r="F48" s="46"/>
       <c r="G48" s="36"/>
@@ -4256,11 +4389,11 @@
       <c r="AP48" s="35"/>
       <c r="AQ48" s="39"/>
     </row>
-    <row r="49" spans="1:50" ht="28.25" customHeight="1" thickBot="1">
+    <row r="49" spans="1:50" ht="28.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A49" s="49"/>
       <c r="B49" s="71"/>
       <c r="C49" s="77"/>
-      <c r="D49" s="21"/>
+      <c r="D49" s="213"/>
       <c r="E49" s="47"/>
       <c r="F49" s="47"/>
       <c r="G49" s="40"/>
@@ -4301,7 +4434,7 @@
       <c r="AP49" s="35"/>
       <c r="AQ49" s="43"/>
     </row>
-    <row r="50" spans="1:50" ht="28.25" customHeight="1" thickBot="1">
+    <row r="50" spans="1:50" ht="28.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A50" s="13"/>
       <c r="B50" s="13"/>
       <c r="C50" s="13"/>
@@ -4346,13 +4479,13 @@
       <c r="AP50" s="35"/>
       <c r="AQ50" s="54"/>
     </row>
-    <row r="51" spans="1:50" ht="17.25" customHeight="1" thickBot="1">
-      <c r="A51" s="177" t="s">
+    <row r="51" spans="1:50" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="178" t="s">
+        <v>51</v>
+      </c>
+      <c r="B51" s="179"/>
+      <c r="C51" s="93" t="s">
         <v>52</v>
-      </c>
-      <c r="B51" s="178"/>
-      <c r="C51" s="93" t="s">
-        <v>53</v>
       </c>
       <c r="D51" s="94"/>
       <c r="E51" s="78"/>
@@ -4396,35 +4529,35 @@
       <c r="AE51" s="80"/>
       <c r="AF51" s="80"/>
       <c r="AG51" s="80"/>
-      <c r="AH51" s="177" t="s">
-        <v>52</v>
-      </c>
-      <c r="AI51" s="194"/>
-      <c r="AJ51" s="194"/>
-      <c r="AK51" s="194"/>
-      <c r="AL51" s="194"/>
-      <c r="AM51" s="194"/>
-      <c r="AN51" s="178"/>
+      <c r="AH51" s="178" t="s">
+        <v>51</v>
+      </c>
+      <c r="AI51" s="195"/>
+      <c r="AJ51" s="195"/>
+      <c r="AK51" s="195"/>
+      <c r="AL51" s="195"/>
+      <c r="AM51" s="195"/>
+      <c r="AN51" s="179"/>
       <c r="AO51" s="85" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="AP51" s="85"/>
       <c r="AQ51" s="100"/>
     </row>
-    <row r="52" spans="1:50" ht="17.25" customHeight="1" thickBot="1">
-      <c r="A52" s="179"/>
-      <c r="B52" s="180"/>
+    <row r="52" spans="1:50" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="180"/>
+      <c r="B52" s="181"/>
       <c r="C52" s="95"/>
       <c r="D52" s="96"/>
       <c r="E52" s="82"/>
       <c r="F52" s="82"/>
-      <c r="G52" s="183">
+      <c r="G52" s="184">
         <f>G51+H51+J51</f>
         <v>0</v>
       </c>
-      <c r="H52" s="184"/>
-      <c r="I52" s="184"/>
-      <c r="J52" s="185"/>
+      <c r="H52" s="185"/>
+      <c r="I52" s="185"/>
+      <c r="J52" s="186"/>
       <c r="K52" s="82"/>
       <c r="L52" s="82"/>
       <c r="M52" s="82"/>
@@ -4448,13 +4581,13 @@
       <c r="AE52" s="2"/>
       <c r="AF52" s="2"/>
       <c r="AG52" s="2"/>
-      <c r="AH52" s="179"/>
-      <c r="AI52" s="195"/>
-      <c r="AJ52" s="195"/>
-      <c r="AK52" s="195"/>
-      <c r="AL52" s="195"/>
-      <c r="AM52" s="195"/>
-      <c r="AN52" s="180"/>
+      <c r="AH52" s="180"/>
+      <c r="AI52" s="196"/>
+      <c r="AJ52" s="196"/>
+      <c r="AK52" s="196"/>
+      <c r="AL52" s="196"/>
+      <c r="AM52" s="196"/>
+      <c r="AN52" s="181"/>
       <c r="AO52" s="86" t="s">
         <v>41</v>
       </c>
@@ -4464,9 +4597,9 @@
       <c r="AU52" s="16"/>
       <c r="AV52" s="16"/>
     </row>
-    <row r="53" spans="1:50" ht="17.25" customHeight="1">
-      <c r="A53" s="179"/>
-      <c r="B53" s="180"/>
+    <row r="53" spans="1:50" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="180"/>
+      <c r="B53" s="181"/>
       <c r="C53" s="93"/>
       <c r="D53" s="94"/>
       <c r="E53" s="82"/>
@@ -4498,22 +4631,22 @@
       <c r="AE53" s="2"/>
       <c r="AF53" s="2"/>
       <c r="AG53" s="2"/>
-      <c r="AH53" s="179"/>
-      <c r="AI53" s="195"/>
-      <c r="AJ53" s="195"/>
-      <c r="AK53" s="195"/>
-      <c r="AL53" s="195"/>
-      <c r="AM53" s="195"/>
-      <c r="AN53" s="180"/>
+      <c r="AH53" s="180"/>
+      <c r="AI53" s="196"/>
+      <c r="AJ53" s="196"/>
+      <c r="AK53" s="196"/>
+      <c r="AL53" s="196"/>
+      <c r="AM53" s="196"/>
+      <c r="AN53" s="181"/>
       <c r="AO53" s="87" t="s">
         <v>33</v>
       </c>
       <c r="AP53" s="87"/>
       <c r="AQ53" s="101"/>
     </row>
-    <row r="54" spans="1:50" ht="17.25" customHeight="1" thickBot="1">
-      <c r="A54" s="181"/>
-      <c r="B54" s="182"/>
+    <row r="54" spans="1:50" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="182"/>
+      <c r="B54" s="183"/>
       <c r="C54" s="97"/>
       <c r="D54" s="98"/>
       <c r="E54" s="82"/>
@@ -4545,13 +4678,13 @@
       <c r="AE54" s="2"/>
       <c r="AF54" s="2"/>
       <c r="AG54" s="2"/>
-      <c r="AH54" s="181"/>
-      <c r="AI54" s="196"/>
-      <c r="AJ54" s="196"/>
-      <c r="AK54" s="196"/>
-      <c r="AL54" s="196"/>
-      <c r="AM54" s="196"/>
-      <c r="AN54" s="182"/>
+      <c r="AH54" s="182"/>
+      <c r="AI54" s="197"/>
+      <c r="AJ54" s="197"/>
+      <c r="AK54" s="197"/>
+      <c r="AL54" s="197"/>
+      <c r="AM54" s="197"/>
+      <c r="AN54" s="183"/>
       <c r="AO54" s="88"/>
       <c r="AP54" s="88"/>
       <c r="AQ54" s="102" t="str">
@@ -4559,7 +4692,7 @@
         <v/>
       </c>
     </row>
-    <row r="55" spans="1:50" ht="17.25" customHeight="1">
+    <row r="55" spans="1:50" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="2"/>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
@@ -4604,7 +4737,7 @@
       <c r="AP55" s="89"/>
       <c r="AQ55" s="2"/>
     </row>
-    <row r="58" spans="1:50" ht="25.25" customHeight="1">
+    <row r="58" spans="1:50" ht="25.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="90"/>
       <c r="B58" s="90"/>
       <c r="C58" s="90"/>
@@ -4612,18 +4745,18 @@
       <c r="E58" s="1"/>
       <c r="F58" s="1"/>
       <c r="G58" s="90"/>
-      <c r="H58" s="190" t="s">
+      <c r="H58" s="191" t="s">
         <v>7</v>
       </c>
-      <c r="I58" s="191"/>
-      <c r="J58" s="191"/>
-      <c r="K58" s="191"/>
-      <c r="L58" s="191"/>
-      <c r="M58" s="191"/>
-      <c r="N58" s="191"/>
-      <c r="O58" s="191"/>
-      <c r="P58" s="192"/>
-      <c r="Q58" s="193"/>
+      <c r="I58" s="192"/>
+      <c r="J58" s="192"/>
+      <c r="K58" s="192"/>
+      <c r="L58" s="192"/>
+      <c r="M58" s="192"/>
+      <c r="N58" s="192"/>
+      <c r="O58" s="192"/>
+      <c r="P58" s="193"/>
+      <c r="Q58" s="194"/>
       <c r="R58" s="82"/>
       <c r="S58" s="82"/>
       <c r="T58" s="82"/>
@@ -4653,7 +4786,7 @@
       <c r="AR58" s="82"/>
       <c r="AS58" s="16"/>
     </row>
-    <row r="59" spans="1:50" s="16" customFormat="1" ht="5" customHeight="1">
+    <row r="59" spans="1:50" s="16" customFormat="1" ht="5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="91"/>
       <c r="B59" s="91"/>
       <c r="C59" s="91"/>
@@ -4704,7 +4837,7 @@
       <c r="AW59"/>
       <c r="AX59"/>
     </row>
-    <row r="60" spans="1:50" s="16" customFormat="1" ht="25.25" customHeight="1">
+    <row r="60" spans="1:50" s="16" customFormat="1" ht="25.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60"/>
       <c r="B60"/>
       <c r="C60"/>
@@ -4712,18 +4845,18 @@
       <c r="E60"/>
       <c r="F60"/>
       <c r="G60"/>
-      <c r="H60" s="190" t="s">
+      <c r="H60" s="191" t="s">
         <v>19</v>
       </c>
-      <c r="I60" s="191"/>
-      <c r="J60" s="191"/>
-      <c r="K60" s="191"/>
-      <c r="L60" s="191"/>
-      <c r="M60" s="191"/>
-      <c r="N60" s="191"/>
-      <c r="O60" s="191"/>
-      <c r="P60" s="192"/>
-      <c r="Q60" s="193"/>
+      <c r="I60" s="192"/>
+      <c r="J60" s="192"/>
+      <c r="K60" s="192"/>
+      <c r="L60" s="192"/>
+      <c r="M60" s="192"/>
+      <c r="N60" s="192"/>
+      <c r="O60" s="192"/>
+      <c r="P60" s="193"/>
+      <c r="Q60" s="194"/>
       <c r="R60"/>
       <c r="S60"/>
       <c r="T60"/>
@@ -4842,12 +4975,12 @@
     <mergeCell ref="P19:Q19"/>
   </mergeCells>
   <conditionalFormatting sqref="AP54">
-    <cfRule type="expression" dxfId="2" priority="14">
+    <cfRule type="expression" dxfId="15" priority="18">
       <formula>AND(ISNUMBER(AP54),OR(AP54&lt;40%,AP54&gt;60%))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AQ54">
-    <cfRule type="expression" dxfId="1" priority="5">
+    <cfRule type="expression" dxfId="14" priority="9">
       <formula>AND(ISNUMBER(AQ54),OR(AQ54&lt;40%,AQ54&gt;60%))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4884,11 +5017,11 @@
   </sheetPr>
   <dimension ref="A1:AV60"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="112" zoomScaleNormal="55" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20:J21"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B31" zoomScale="112" zoomScaleNormal="55" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22:D49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="12" customWidth="1"/>
     <col min="3" max="3" width="50.33203125" customWidth="1"/>
@@ -4901,7 +5034,7 @@
     <col min="42" max="46" width="11.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" ht="17" customHeight="1" thickBot="1">
+    <row r="1" spans="1:42" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="G1" s="144" t="s">
         <v>0</v>
       </c>
@@ -4943,7 +5076,7 @@
       <c r="AO1" s="104"/>
       <c r="AP1" s="103"/>
     </row>
-    <row r="2" spans="1:42" ht="17" customHeight="1" thickBot="1">
+    <row r="2" spans="1:42" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="G2" s="144" t="s">
         <v>6</v>
       </c>
@@ -4953,7 +5086,7 @@
       <c r="K2" s="145"/>
       <c r="L2" s="146"/>
       <c r="M2" s="144" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="N2" s="145"/>
       <c r="O2" s="145"/>
@@ -4964,7 +5097,7 @@
       <c r="T2" s="145"/>
       <c r="U2" s="146"/>
     </row>
-    <row r="3" spans="1:42" ht="17" customHeight="1" thickBot="1">
+    <row r="3" spans="1:42" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="G3" s="144" t="s">
         <v>5</v>
       </c>
@@ -4974,7 +5107,7 @@
       <c r="K3" s="145"/>
       <c r="L3" s="146"/>
       <c r="M3" s="144" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="N3" s="145"/>
       <c r="O3" s="145"/>
@@ -4985,7 +5118,7 @@
       <c r="T3" s="145"/>
       <c r="U3" s="146"/>
     </row>
-    <row r="4" spans="1:42" ht="17" customHeight="1" thickBot="1">
+    <row r="4" spans="1:42" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="G4" s="144" t="s">
         <v>20</v>
       </c>
@@ -5006,7 +5139,7 @@
       <c r="T4" s="145"/>
       <c r="U4" s="146"/>
     </row>
-    <row r="5" spans="1:42" ht="17" customHeight="1" thickBot="1">
+    <row r="5" spans="1:42" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="G5" s="144" t="s">
         <v>8</v>
       </c>
@@ -5027,7 +5160,7 @@
       <c r="T5" s="145"/>
       <c r="U5" s="146"/>
     </row>
-    <row r="6" spans="1:42" ht="17" customHeight="1" thickBot="1">
+    <row r="6" spans="1:42" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D6" s="105" t="s">
         <v>47</v>
       </c>
@@ -5051,7 +5184,7 @@
       <c r="T6" s="145"/>
       <c r="U6" s="146"/>
     </row>
-    <row r="7" spans="1:42" ht="17" customHeight="1">
+    <row r="7" spans="1:42" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="106"/>
       <c r="B7" s="106"/>
       <c r="C7" s="106"/>
@@ -5088,7 +5221,7 @@
       <c r="AJ7" s="106"/>
       <c r="AK7" s="106"/>
     </row>
-    <row r="8" spans="1:42" ht="15.5" customHeight="1">
+    <row r="8" spans="1:42" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="107" t="s">
         <v>18</v>
       </c>
@@ -5117,7 +5250,7 @@
       <c r="AJ8" s="106"/>
       <c r="AK8" s="106"/>
     </row>
-    <row r="9" spans="1:42" ht="5" customHeight="1">
+    <row r="9" spans="1:42" ht="5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="103"/>
       <c r="B9" s="103"/>
       <c r="C9" s="103"/>
@@ -5159,7 +5292,7 @@
       <c r="AO9" s="104"/>
       <c r="AP9" s="106"/>
     </row>
-    <row r="10" spans="1:42" ht="15.5" customHeight="1">
+    <row r="10" spans="1:42" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="90"/>
       <c r="B10" s="90"/>
       <c r="C10" s="90"/>
@@ -5185,7 +5318,7 @@
       <c r="T10" s="112"/>
       <c r="U10" s="112"/>
     </row>
-    <row r="11" spans="1:42" ht="5" customHeight="1">
+    <row r="11" spans="1:42" ht="5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -5193,17 +5326,17 @@
       <c r="E11" s="24"/>
       <c r="F11" s="11"/>
     </row>
-    <row r="12" spans="1:42" ht="15.5" customHeight="1">
+    <row r="12" spans="1:42" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E12" s="22"/>
       <c r="F12" s="107" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:42" ht="5" customHeight="1">
+    <row r="13" spans="1:42" ht="5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E13" s="109"/>
       <c r="F13" s="107"/>
     </row>
-    <row r="14" spans="1:42" ht="15.5" customHeight="1">
+    <row r="14" spans="1:42" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -5213,15 +5346,15 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:42" ht="11" customHeight="1" thickBot="1">
-      <c r="A15" s="208"/>
-      <c r="B15" s="208"/>
-      <c r="C15" s="208"/>
-      <c r="D15" s="208"/>
+    <row r="15" spans="1:42" ht="11" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="209"/>
+      <c r="B15" s="209"/>
+      <c r="C15" s="209"/>
+      <c r="D15" s="209"/>
       <c r="E15" s="16"/>
       <c r="F15" s="16"/>
     </row>
-    <row r="16" spans="1:42" ht="24.75" customHeight="1" thickBot="1">
+    <row r="16" spans="1:42" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="16"/>
       <c r="B16" s="16"/>
       <c r="C16" s="16"/>
@@ -5261,7 +5394,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:41" ht="24.75" customHeight="1" thickBot="1">
+    <row r="17" spans="1:41" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="16"/>
       <c r="B17" s="16"/>
       <c r="C17" s="16"/>
@@ -5303,7 +5436,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:41" ht="45.75" customHeight="1" thickBot="1">
+    <row r="18" spans="1:41" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="16"/>
       <c r="B18" s="16"/>
       <c r="C18" s="16"/>
@@ -5345,9 +5478,9 @@
       <c r="AL18" s="141"/>
       <c r="AM18" s="142"/>
       <c r="AN18" s="113"/>
-      <c r="AO18" s="168"/>
-    </row>
-    <row r="19" spans="1:41" s="2" customFormat="1" ht="45.75" customHeight="1" thickBot="1">
+      <c r="AO18" s="169"/>
+    </row>
+    <row r="19" spans="1:41" s="2" customFormat="1" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="127" t="s">
         <v>17</v>
       </c>
@@ -5367,7 +5500,7 @@
       </c>
       <c r="L19" s="156"/>
       <c r="M19" s="156"/>
-      <c r="N19" s="163" t="s">
+      <c r="N19" s="164" t="s">
         <v>24</v>
       </c>
       <c r="O19" s="143"/>
@@ -5382,7 +5515,7 @@
       <c r="T19" s="143" t="s">
         <v>27</v>
       </c>
-      <c r="U19" s="173"/>
+      <c r="U19" s="174"/>
       <c r="V19" s="143" t="s">
         <v>25</v>
       </c>
@@ -5395,10 +5528,10 @@
         <v>38</v>
       </c>
       <c r="AA19" s="130"/>
-      <c r="AB19" s="171" t="s">
+      <c r="AB19" s="172" t="s">
         <v>34</v>
       </c>
-      <c r="AC19" s="172"/>
+      <c r="AC19" s="173"/>
       <c r="AD19" s="130" t="s">
         <v>26</v>
       </c>
@@ -5420,20 +5553,20 @@
       </c>
       <c r="AM19" s="131"/>
       <c r="AN19" s="109"/>
-      <c r="AO19" s="169"/>
-    </row>
-    <row r="20" spans="1:41" ht="22.5" customHeight="1">
-      <c r="A20" s="164" t="s">
+      <c r="AO19" s="170"/>
+    </row>
+    <row r="20" spans="1:41" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="165" t="s">
         <v>50</v>
       </c>
-      <c r="B20" s="187" t="s">
+      <c r="B20" s="188" t="s">
         <v>10</v>
       </c>
-      <c r="C20" s="166" t="s">
+      <c r="C20" s="167" t="s">
         <v>9</v>
       </c>
-      <c r="D20" s="166" t="s">
-        <v>51</v>
+      <c r="D20" s="167" t="s">
+        <v>60</v>
       </c>
       <c r="E20" s="150" t="s">
         <v>48</v>
@@ -5447,22 +5580,22 @@
       <c r="H20" s="157" t="s">
         <v>3</v>
       </c>
-      <c r="I20" s="188" t="s">
+      <c r="I20" s="189" t="s">
         <v>4</v>
       </c>
-      <c r="J20" s="209" t="s">
-        <v>60</v>
-      </c>
-      <c r="K20" s="160" t="s">
+      <c r="J20" s="159" t="s">
+        <v>59</v>
+      </c>
+      <c r="K20" s="161" t="s">
         <v>2</v>
       </c>
-      <c r="L20" s="189" t="s">
+      <c r="L20" s="190" t="s">
         <v>3</v>
       </c>
-      <c r="M20" s="186" t="s">
+      <c r="M20" s="187" t="s">
         <v>4</v>
       </c>
-      <c r="N20" s="161" t="s">
+      <c r="N20" s="162" t="s">
         <v>30</v>
       </c>
       <c r="O20" s="133" t="s">
@@ -5486,7 +5619,7 @@
       <c r="U20" s="135" t="s">
         <v>31</v>
       </c>
-      <c r="V20" s="161" t="s">
+      <c r="V20" s="162" t="s">
         <v>30</v>
       </c>
       <c r="W20" s="133" t="s">
@@ -5498,7 +5631,7 @@
       <c r="Y20" s="135" t="s">
         <v>31</v>
       </c>
-      <c r="Z20" s="161" t="s">
+      <c r="Z20" s="162" t="s">
         <v>30</v>
       </c>
       <c r="AA20" s="133" t="s">
@@ -5522,7 +5655,7 @@
       <c r="AG20" s="135" t="s">
         <v>31</v>
       </c>
-      <c r="AH20" s="161" t="s">
+      <c r="AH20" s="162" t="s">
         <v>30</v>
       </c>
       <c r="AI20" s="133" t="s">
@@ -5541,23 +5674,23 @@
         <v>31</v>
       </c>
       <c r="AN20" s="114"/>
-      <c r="AO20" s="169"/>
-    </row>
-    <row r="21" spans="1:41" ht="22.5" customHeight="1" thickBot="1">
-      <c r="A21" s="165"/>
-      <c r="B21" s="165"/>
-      <c r="C21" s="167"/>
-      <c r="D21" s="167"/>
+      <c r="AO20" s="170"/>
+    </row>
+    <row r="21" spans="1:41" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="166"/>
+      <c r="B21" s="166"/>
+      <c r="C21" s="168"/>
+      <c r="D21" s="168"/>
       <c r="E21" s="151"/>
       <c r="F21" s="151"/>
       <c r="G21" s="154"/>
       <c r="H21" s="158"/>
       <c r="I21" s="158"/>
-      <c r="J21" s="159"/>
+      <c r="J21" s="160"/>
       <c r="K21" s="154"/>
       <c r="L21" s="158"/>
-      <c r="M21" s="159"/>
-      <c r="N21" s="162"/>
+      <c r="M21" s="160"/>
+      <c r="N21" s="163"/>
       <c r="O21" s="134"/>
       <c r="P21" s="134"/>
       <c r="Q21" s="134"/>
@@ -5565,11 +5698,11 @@
       <c r="S21" s="134"/>
       <c r="T21" s="134"/>
       <c r="U21" s="136"/>
-      <c r="V21" s="162"/>
+      <c r="V21" s="163"/>
       <c r="W21" s="134"/>
       <c r="X21" s="134"/>
       <c r="Y21" s="136"/>
-      <c r="Z21" s="162"/>
+      <c r="Z21" s="163"/>
       <c r="AA21" s="134"/>
       <c r="AB21" s="134"/>
       <c r="AC21" s="134"/>
@@ -5577,16 +5710,16 @@
       <c r="AE21" s="134"/>
       <c r="AF21" s="134"/>
       <c r="AG21" s="136"/>
-      <c r="AH21" s="162"/>
+      <c r="AH21" s="163"/>
       <c r="AI21" s="134"/>
       <c r="AJ21" s="134"/>
       <c r="AK21" s="134"/>
       <c r="AL21" s="134"/>
       <c r="AM21" s="136"/>
       <c r="AN21" s="114"/>
-      <c r="AO21" s="170"/>
-    </row>
-    <row r="22" spans="1:41" ht="28.25" customHeight="1">
+      <c r="AO21" s="171"/>
+    </row>
+    <row r="22" spans="1:41" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="51"/>
       <c r="B22" s="69"/>
       <c r="C22" s="75"/>
@@ -5629,7 +5762,7 @@
       <c r="AN22" s="80"/>
       <c r="AO22" s="92"/>
     </row>
-    <row r="23" spans="1:41" ht="27.75" customHeight="1">
+    <row r="23" spans="1:41" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="48"/>
       <c r="B23" s="70"/>
       <c r="C23" s="76"/>
@@ -5672,7 +5805,7 @@
       <c r="AN23" s="80"/>
       <c r="AO23" s="39"/>
     </row>
-    <row r="24" spans="1:41" ht="28.25" customHeight="1">
+    <row r="24" spans="1:41" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="48"/>
       <c r="B24" s="70"/>
       <c r="C24" s="76"/>
@@ -5715,7 +5848,7 @@
       <c r="AN24" s="80"/>
       <c r="AO24" s="39"/>
     </row>
-    <row r="25" spans="1:41" ht="28.25" customHeight="1">
+    <row r="25" spans="1:41" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="48"/>
       <c r="B25" s="70"/>
       <c r="C25" s="76"/>
@@ -5758,7 +5891,7 @@
       <c r="AN25" s="80"/>
       <c r="AO25" s="39"/>
     </row>
-    <row r="26" spans="1:41" ht="27.75" customHeight="1">
+    <row r="26" spans="1:41" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="48"/>
       <c r="B26" s="70"/>
       <c r="C26" s="76"/>
@@ -5801,7 +5934,7 @@
       <c r="AN26" s="80"/>
       <c r="AO26" s="39"/>
     </row>
-    <row r="27" spans="1:41" ht="28.25" customHeight="1">
+    <row r="27" spans="1:41" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="48"/>
       <c r="B27" s="70"/>
       <c r="C27" s="76"/>
@@ -5844,7 +5977,7 @@
       <c r="AN27" s="80"/>
       <c r="AO27" s="39"/>
     </row>
-    <row r="28" spans="1:41" ht="27.75" customHeight="1">
+    <row r="28" spans="1:41" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="48"/>
       <c r="B28" s="70"/>
       <c r="C28" s="76"/>
@@ -5887,7 +6020,7 @@
       <c r="AN28" s="80"/>
       <c r="AO28" s="39"/>
     </row>
-    <row r="29" spans="1:41" ht="28.25" customHeight="1">
+    <row r="29" spans="1:41" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="48"/>
       <c r="B29" s="70"/>
       <c r="C29" s="76"/>
@@ -5930,7 +6063,7 @@
       <c r="AN29" s="80"/>
       <c r="AO29" s="39"/>
     </row>
-    <row r="30" spans="1:41" ht="28.25" customHeight="1">
+    <row r="30" spans="1:41" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="48"/>
       <c r="B30" s="70"/>
       <c r="C30" s="76"/>
@@ -5973,7 +6106,7 @@
       <c r="AN30" s="80"/>
       <c r="AO30" s="39"/>
     </row>
-    <row r="31" spans="1:41" ht="28.25" customHeight="1">
+    <row r="31" spans="1:41" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="48"/>
       <c r="B31" s="70"/>
       <c r="C31" s="76"/>
@@ -6016,7 +6149,7 @@
       <c r="AN31" s="80"/>
       <c r="AO31" s="39"/>
     </row>
-    <row r="32" spans="1:41" ht="28.25" customHeight="1">
+    <row r="32" spans="1:41" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="48"/>
       <c r="B32" s="70"/>
       <c r="C32" s="76"/>
@@ -6059,7 +6192,7 @@
       <c r="AN32" s="80"/>
       <c r="AO32" s="39"/>
     </row>
-    <row r="33" spans="1:41" ht="28.25" customHeight="1">
+    <row r="33" spans="1:41" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="48"/>
       <c r="B33" s="70"/>
       <c r="C33" s="76"/>
@@ -6102,7 +6235,7 @@
       <c r="AN33" s="80"/>
       <c r="AO33" s="39"/>
     </row>
-    <row r="34" spans="1:41" ht="28.25" customHeight="1">
+    <row r="34" spans="1:41" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="48"/>
       <c r="B34" s="70"/>
       <c r="C34" s="76"/>
@@ -6145,7 +6278,7 @@
       <c r="AN34" s="80"/>
       <c r="AO34" s="39"/>
     </row>
-    <row r="35" spans="1:41" ht="28.25" customHeight="1">
+    <row r="35" spans="1:41" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="48"/>
       <c r="B35" s="70"/>
       <c r="C35" s="76"/>
@@ -6188,7 +6321,7 @@
       <c r="AN35" s="80"/>
       <c r="AO35" s="39"/>
     </row>
-    <row r="36" spans="1:41" ht="28.25" customHeight="1">
+    <row r="36" spans="1:41" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="48"/>
       <c r="B36" s="70"/>
       <c r="C36" s="76"/>
@@ -6231,7 +6364,7 @@
       <c r="AN36" s="80"/>
       <c r="AO36" s="39"/>
     </row>
-    <row r="37" spans="1:41" ht="28.25" customHeight="1">
+    <row r="37" spans="1:41" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="48"/>
       <c r="B37" s="70"/>
       <c r="C37" s="76"/>
@@ -6274,7 +6407,7 @@
       <c r="AN37" s="80"/>
       <c r="AO37" s="39"/>
     </row>
-    <row r="38" spans="1:41" ht="28.25" customHeight="1">
+    <row r="38" spans="1:41" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="48"/>
       <c r="B38" s="70"/>
       <c r="C38" s="76"/>
@@ -6317,7 +6450,7 @@
       <c r="AN38" s="80"/>
       <c r="AO38" s="39"/>
     </row>
-    <row r="39" spans="1:41" ht="28.25" customHeight="1">
+    <row r="39" spans="1:41" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="48"/>
       <c r="B39" s="70"/>
       <c r="C39" s="76"/>
@@ -6360,7 +6493,7 @@
       <c r="AN39" s="80"/>
       <c r="AO39" s="39"/>
     </row>
-    <row r="40" spans="1:41" ht="28.25" customHeight="1">
+    <row r="40" spans="1:41" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="48"/>
       <c r="B40" s="70"/>
       <c r="C40" s="76"/>
@@ -6403,7 +6536,7 @@
       <c r="AN40" s="80"/>
       <c r="AO40" s="39"/>
     </row>
-    <row r="41" spans="1:41" ht="28.25" customHeight="1">
+    <row r="41" spans="1:41" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="48"/>
       <c r="B41" s="70"/>
       <c r="C41" s="76"/>
@@ -6446,7 +6579,7 @@
       <c r="AN41" s="80"/>
       <c r="AO41" s="39"/>
     </row>
-    <row r="42" spans="1:41" ht="28.25" customHeight="1">
+    <row r="42" spans="1:41" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="12"/>
       <c r="B42" s="70"/>
       <c r="C42" s="76"/>
@@ -6489,7 +6622,7 @@
       <c r="AN42" s="80"/>
       <c r="AO42" s="39"/>
     </row>
-    <row r="43" spans="1:41" ht="28.25" customHeight="1">
+    <row r="43" spans="1:41" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="48"/>
       <c r="B43" s="70"/>
       <c r="C43" s="76"/>
@@ -6532,7 +6665,7 @@
       <c r="AN43" s="80"/>
       <c r="AO43" s="39"/>
     </row>
-    <row r="44" spans="1:41" ht="28.25" customHeight="1">
+    <row r="44" spans="1:41" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="12"/>
       <c r="B44" s="70"/>
       <c r="C44" s="76"/>
@@ -6575,7 +6708,7 @@
       <c r="AN44" s="80"/>
       <c r="AO44" s="39"/>
     </row>
-    <row r="45" spans="1:41" ht="28.25" customHeight="1">
+    <row r="45" spans="1:41" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="48"/>
       <c r="B45" s="70"/>
       <c r="C45" s="76"/>
@@ -6618,7 +6751,7 @@
       <c r="AN45" s="80"/>
       <c r="AO45" s="39"/>
     </row>
-    <row r="46" spans="1:41" ht="28.25" customHeight="1">
+    <row r="46" spans="1:41" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="12"/>
       <c r="B46" s="70"/>
       <c r="C46" s="76"/>
@@ -6661,7 +6794,7 @@
       <c r="AN46" s="80"/>
       <c r="AO46" s="39"/>
     </row>
-    <row r="47" spans="1:41" ht="28.25" customHeight="1">
+    <row r="47" spans="1:41" ht="28.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="48"/>
       <c r="B47" s="70"/>
       <c r="C47" s="76"/>
@@ -6704,7 +6837,7 @@
       <c r="AN47" s="80"/>
       <c r="AO47" s="39"/>
     </row>
-    <row r="48" spans="1:41" ht="27.75" customHeight="1">
+    <row r="48" spans="1:41" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="12"/>
       <c r="B48" s="70"/>
       <c r="C48" s="76"/>
@@ -6747,7 +6880,7 @@
       <c r="AN48" s="80"/>
       <c r="AO48" s="39"/>
     </row>
-    <row r="49" spans="1:48" ht="28.25" customHeight="1" thickBot="1">
+    <row r="49" spans="1:48" ht="28.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A49" s="49"/>
       <c r="B49" s="71"/>
       <c r="C49" s="77"/>
@@ -6790,7 +6923,7 @@
       <c r="AN49" s="80"/>
       <c r="AO49" s="43"/>
     </row>
-    <row r="50" spans="1:48" ht="28.25" customHeight="1" thickBot="1">
+    <row r="50" spans="1:48" ht="28.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A50" s="125"/>
       <c r="B50" s="125"/>
       <c r="C50" s="125"/>
@@ -6833,15 +6966,15 @@
       <c r="AN50" s="80"/>
       <c r="AO50" s="126"/>
     </row>
-    <row r="51" spans="1:48" ht="17.25" customHeight="1" thickBot="1">
-      <c r="A51" s="177" t="s">
-        <v>59</v>
-      </c>
-      <c r="B51" s="178"/>
-      <c r="C51" s="197" t="s">
-        <v>53</v>
-      </c>
-      <c r="D51" s="198"/>
+    <row r="51" spans="1:48" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="178" t="s">
+        <v>58</v>
+      </c>
+      <c r="B51" s="179"/>
+      <c r="C51" s="198" t="s">
+        <v>52</v>
+      </c>
+      <c r="D51" s="199"/>
       <c r="E51" s="78"/>
       <c r="F51" s="78"/>
       <c r="G51" s="79">
@@ -6883,33 +7016,33 @@
       <c r="AE51" s="80"/>
       <c r="AF51" s="80"/>
       <c r="AG51" s="80"/>
-      <c r="AH51" s="177" t="s">
-        <v>59</v>
-      </c>
-      <c r="AI51" s="194"/>
-      <c r="AJ51" s="194"/>
-      <c r="AK51" s="194"/>
-      <c r="AL51" s="202" t="s">
-        <v>54</v>
-      </c>
-      <c r="AM51" s="203"/>
-      <c r="AN51" s="204"/>
+      <c r="AH51" s="178" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI51" s="195"/>
+      <c r="AJ51" s="195"/>
+      <c r="AK51" s="195"/>
+      <c r="AL51" s="203" t="s">
+        <v>53</v>
+      </c>
+      <c r="AM51" s="204"/>
+      <c r="AN51" s="205"/>
       <c r="AO51" s="100"/>
     </row>
-    <row r="52" spans="1:48" ht="17.25" customHeight="1" thickBot="1">
-      <c r="A52" s="179"/>
-      <c r="B52" s="180"/>
-      <c r="C52" s="199"/>
-      <c r="D52" s="200"/>
+    <row r="52" spans="1:48" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="180"/>
+      <c r="B52" s="181"/>
+      <c r="C52" s="200"/>
+      <c r="D52" s="201"/>
       <c r="E52" s="82"/>
       <c r="F52" s="82"/>
-      <c r="G52" s="183">
+      <c r="G52" s="184">
         <f>G51+H51+J51</f>
         <v>0</v>
       </c>
-      <c r="H52" s="184"/>
-      <c r="I52" s="184"/>
-      <c r="J52" s="185"/>
+      <c r="H52" s="185"/>
+      <c r="I52" s="185"/>
+      <c r="J52" s="186"/>
       <c r="K52" s="82"/>
       <c r="L52" s="82"/>
       <c r="M52" s="82"/>
@@ -6933,15 +7066,15 @@
       <c r="AE52" s="2"/>
       <c r="AF52" s="2"/>
       <c r="AG52" s="2"/>
-      <c r="AH52" s="179"/>
-      <c r="AI52" s="201"/>
-      <c r="AJ52" s="201"/>
-      <c r="AK52" s="201"/>
-      <c r="AL52" s="205" t="s">
+      <c r="AH52" s="180"/>
+      <c r="AI52" s="202"/>
+      <c r="AJ52" s="202"/>
+      <c r="AK52" s="202"/>
+      <c r="AL52" s="206" t="s">
         <v>41</v>
       </c>
-      <c r="AM52" s="206"/>
-      <c r="AN52" s="207"/>
+      <c r="AM52" s="207"/>
+      <c r="AN52" s="208"/>
       <c r="AO52" s="84">
         <f>SUM(AO22:AO49)</f>
         <v>0</v>
@@ -6950,9 +7083,9 @@
       <c r="AS52" s="16"/>
       <c r="AT52" s="16"/>
     </row>
-    <row r="53" spans="1:48" ht="17.25" customHeight="1">
-      <c r="A53" s="179"/>
-      <c r="B53" s="180"/>
+    <row r="53" spans="1:48" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="180"/>
+      <c r="B53" s="181"/>
       <c r="C53" s="93"/>
       <c r="D53" s="94"/>
       <c r="E53" s="82"/>
@@ -6984,20 +7117,20 @@
       <c r="AE53" s="2"/>
       <c r="AF53" s="2"/>
       <c r="AG53" s="2"/>
-      <c r="AH53" s="179"/>
-      <c r="AI53" s="201"/>
-      <c r="AJ53" s="201"/>
-      <c r="AK53" s="201"/>
-      <c r="AL53" s="177" t="s">
+      <c r="AH53" s="180"/>
+      <c r="AI53" s="202"/>
+      <c r="AJ53" s="202"/>
+      <c r="AK53" s="202"/>
+      <c r="AL53" s="178" t="s">
         <v>33</v>
       </c>
-      <c r="AM53" s="194"/>
-      <c r="AN53" s="178"/>
+      <c r="AM53" s="195"/>
+      <c r="AN53" s="179"/>
       <c r="AO53" s="101"/>
     </row>
-    <row r="54" spans="1:48" ht="17.25" customHeight="1" thickBot="1">
-      <c r="A54" s="181"/>
-      <c r="B54" s="182"/>
+    <row r="54" spans="1:48" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="182"/>
+      <c r="B54" s="183"/>
       <c r="C54" s="97"/>
       <c r="D54" s="98"/>
       <c r="E54" s="82"/>
@@ -7029,19 +7162,19 @@
       <c r="AE54" s="2"/>
       <c r="AF54" s="2"/>
       <c r="AG54" s="2"/>
-      <c r="AH54" s="181"/>
-      <c r="AI54" s="196"/>
-      <c r="AJ54" s="196"/>
-      <c r="AK54" s="196"/>
-      <c r="AL54" s="181"/>
-      <c r="AM54" s="196"/>
-      <c r="AN54" s="182"/>
+      <c r="AH54" s="182"/>
+      <c r="AI54" s="197"/>
+      <c r="AJ54" s="197"/>
+      <c r="AK54" s="197"/>
+      <c r="AL54" s="182"/>
+      <c r="AM54" s="197"/>
+      <c r="AN54" s="183"/>
       <c r="AO54" s="102" t="str">
         <f t="shared" ref="AO54" si="0">IFERROR(AO53/AO52,"")</f>
         <v/>
       </c>
     </row>
-    <row r="55" spans="1:48" ht="17.25" customHeight="1">
+    <row r="55" spans="1:48" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="2"/>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
@@ -7084,7 +7217,7 @@
       <c r="AN55" s="89"/>
       <c r="AO55" s="2"/>
     </row>
-    <row r="58" spans="1:48" ht="25.25" customHeight="1">
+    <row r="58" spans="1:48" ht="25.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="90"/>
       <c r="B58" s="90"/>
       <c r="C58" s="90"/>
@@ -7092,18 +7225,18 @@
       <c r="E58" s="1"/>
       <c r="F58" s="1"/>
       <c r="G58" s="90"/>
-      <c r="H58" s="190" t="s">
+      <c r="H58" s="191" t="s">
         <v>7</v>
       </c>
-      <c r="I58" s="191"/>
-      <c r="J58" s="191"/>
-      <c r="K58" s="191"/>
-      <c r="L58" s="191"/>
-      <c r="M58" s="191"/>
-      <c r="N58" s="191"/>
-      <c r="O58" s="191"/>
-      <c r="P58" s="192"/>
-      <c r="Q58" s="193"/>
+      <c r="I58" s="192"/>
+      <c r="J58" s="192"/>
+      <c r="K58" s="192"/>
+      <c r="L58" s="192"/>
+      <c r="M58" s="192"/>
+      <c r="N58" s="192"/>
+      <c r="O58" s="192"/>
+      <c r="P58" s="193"/>
+      <c r="Q58" s="194"/>
       <c r="R58" s="82"/>
       <c r="S58" s="82"/>
       <c r="T58" s="82"/>
@@ -7131,7 +7264,7 @@
       <c r="AP58" s="82"/>
       <c r="AQ58" s="16"/>
     </row>
-    <row r="59" spans="1:48" s="16" customFormat="1" ht="5" customHeight="1">
+    <row r="59" spans="1:48" s="16" customFormat="1" ht="5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="91"/>
       <c r="B59" s="91"/>
       <c r="C59" s="91"/>
@@ -7180,7 +7313,7 @@
       <c r="AU59"/>
       <c r="AV59"/>
     </row>
-    <row r="60" spans="1:48" s="16" customFormat="1" ht="25.25" customHeight="1">
+    <row r="60" spans="1:48" s="16" customFormat="1" ht="25.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60"/>
       <c r="B60"/>
       <c r="C60"/>
@@ -7188,18 +7321,18 @@
       <c r="E60"/>
       <c r="F60"/>
       <c r="G60"/>
-      <c r="H60" s="190" t="s">
+      <c r="H60" s="191" t="s">
         <v>19</v>
       </c>
-      <c r="I60" s="191"/>
-      <c r="J60" s="191"/>
-      <c r="K60" s="191"/>
-      <c r="L60" s="191"/>
-      <c r="M60" s="191"/>
-      <c r="N60" s="191"/>
-      <c r="O60" s="191"/>
-      <c r="P60" s="192"/>
-      <c r="Q60" s="193"/>
+      <c r="I60" s="192"/>
+      <c r="J60" s="192"/>
+      <c r="K60" s="192"/>
+      <c r="L60" s="192"/>
+      <c r="M60" s="192"/>
+      <c r="N60" s="192"/>
+      <c r="O60" s="192"/>
+      <c r="P60" s="193"/>
+      <c r="Q60" s="194"/>
       <c r="R60"/>
       <c r="S60"/>
       <c r="T60"/>
@@ -7278,6 +7411,8 @@
     <mergeCell ref="AB19:AC19"/>
     <mergeCell ref="AD19:AE19"/>
     <mergeCell ref="AF19:AG19"/>
+    <mergeCell ref="Y20:Y21"/>
+    <mergeCell ref="Z20:Z21"/>
     <mergeCell ref="AH19:AI19"/>
     <mergeCell ref="J20:J21"/>
     <mergeCell ref="K20:K21"/>
@@ -7294,8 +7429,6 @@
     <mergeCell ref="V20:V21"/>
     <mergeCell ref="W20:W21"/>
     <mergeCell ref="X20:X21"/>
-    <mergeCell ref="Y20:Y21"/>
-    <mergeCell ref="Z20:Z21"/>
     <mergeCell ref="AM20:AM21"/>
     <mergeCell ref="AB20:AB21"/>
     <mergeCell ref="AC20:AC21"/>
@@ -7321,7 +7454,7 @@
     <mergeCell ref="C51:D52"/>
   </mergeCells>
   <conditionalFormatting sqref="AO54">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="12" priority="2">
       <formula>AND(ISNUMBER(AO54),OR(AO54&lt;40%,AO54&gt;60%))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>